<commit_message>
Updated API Lists in accordance with V3
</commit_message>
<xml_diff>
--- a/Documentation/001-Requirement/API-List.xlsx
+++ b/Documentation/001-Requirement/API-List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uhgazure-my.sharepoint.com/personal/varenya_varshney_optum_com/Documents/Home/Reference/MTech/Sem1/DatabaseDesignAndApplication/AssignmentRelated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\001-Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{9C69EC02-9CC7-4F69-AEAF-B1B36FC39421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E1AF327-D68E-4756-9828-AB6343DB8EFA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD26C15-8E03-42B4-A051-BF27067CE5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="11724" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Admin</t>
   </si>
@@ -96,69 +96,89 @@
     <t>receiving branch code, shipment_id</t>
   </si>
   <si>
-    <t>Deliver Shipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When a shipment is marked as Out_For_Delivery, an agent from the destination branch attempts the delivery and performs below task:
-1. if delivered -&gt; status = delivered ; else Undelivered with some remarks
-2. Insert row into shipment_history; shipment_id, created_by, created_on, shipment_status
+    <t>shipment_id</t>
+  </si>
+  <si>
+    <t>Track Shipment</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>CRUD Customer</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Serviceable Pincodes</t>
+  </si>
+  <si>
+    <t>CRUD Employee</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Can be skipped. Insert scripts are sufficient</t>
+  </si>
+  <si>
+    <t>Delete can be skipped</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Branch; 1 Stored Proc for Create and Update; While insertign into branch, make sure to insert branch's pincode to service_pincode table as well</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Agent; 1 Stored Proc for Create and Update</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Customer; 1 Stored Proc for Create and Update</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Employee; 1 Stored Proc for Create and Update; Create a sequence to generate employee_id of 6 digits</t>
+  </si>
+  <si>
+    <t>Once the payment is received (offline), Agent receives the shipment and performs below tasks:
+1. Checks if customer is registered looking at his contact_num. If no, then registers the customer. 
+2. A record is inserted into shipment:
+    Update its attributes such that cusotmer_id=regd customer id (source branch and address details can be  determined using customer's address details), dest_branch=branch of dest pincode, next_branch = source_branch; status = booked
+3. Insert a record into shipment_tracker shipment_id; agent_id, current_branch = null; next_branch=source_branch; creation_datetime, status=booked</t>
+  </si>
+  <si>
+    <t>When a shipment is arrived at any branch, employee at the branch will perform below tasks:
+1. Update shipment table with status = RECEIVED_AT_DEST_BRANCH if current_branch = dest_branch else status = IN_TRANSIT
+2. Insert a row into shipment_tracker table by referring to route table:
+ shipment_id; employee_id, current_branch = receiving branch; next_branch=determine from route detail; creation_datetime, status=RECEIVED_AT_DEST_BRANCH or IN_TRANSIT</t>
+  </si>
+  <si>
+    <t>Attempt Delivery</t>
+  </si>
+  <si>
+    <t>Update Delivery Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a shipment is marked as RECEIVED_AT_DEST_BRANCH, an agent from the destination branch attempts the delivery and performs below task:
+1. Updates shipment table such that status = OUT_FOR_DELIVERY
+2. Insert a record into shipment_tracker; shipment_id, agent_id, creation_datetime,status=OUT_FOR_DELIVERY
 </t>
   </si>
   <si>
-    <t>When a shipment is arrived at any branch, agent at the branch will perform below tasks:
-current_branch = branch_code of receiving branch;
-if current_branch == dest branch
-      mark it as Out_For_delivery
-else
-      determine next_branch and transport_mode using route table
-      update status = IN_TRANSIT
-      insert row into shipment_history; shipment_id, received_at, created_by, created_on, shipment_status</t>
-  </si>
-  <si>
-    <t>Once the payment is received (offline), Agent receives the shipment and performs below tasks:
-1. A record is inserted into shipment_details:
-    Update its attributes such that source_branch=branch of source pincode, dest_branch=branch of dest pincode, next_branch = source_branch, current_branch = null.
-    Status = booked
-2. Insert a record in shipment_history shipment_id, created_by, created_on, shipment_status</t>
-  </si>
-  <si>
-    <t>shipment_id</t>
-  </si>
-  <si>
-    <t>Track Shipment</t>
-  </si>
-  <si>
-    <t>At any point in time, customer should be able to track the full history of the shipment. This API would query shipment_details and shipment_history table and produce required output</t>
-  </si>
-  <si>
-    <t>shipment_details and shipment_history</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>CRUD Customer</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>Create, Read, Update, Delete on Branch</t>
-  </si>
-  <si>
-    <t>Create, Read, Update, Delete on Agent</t>
-  </si>
-  <si>
-    <t>Create, Read, Update, Delete on Serviceable Pincodes</t>
-  </si>
-  <si>
-    <t>Create, Read, Update, Delete on Customer</t>
+    <t xml:space="preserve">When a shipment is marked as OUT_FOR_DELIVERY, the same agent from the destination branch updates the status of the delivery and performs below task:
+1. Updates shipment table such that status = DELIVERED or UNDELIVERED and adds status_remarks (optional)
+2. Insert a record into shipment_tracker; shipment_id, agent_id, creation_datetime,status=DELIVERED or UNDELIVERED
+</t>
+  </si>
+  <si>
+    <t>At any point in time, customer should be able to track the full history of the shipment. This API would query shipment_tracker table and produce required output</t>
+  </si>
+  <si>
+    <t>shipment and shipment_tracker</t>
   </si>
 </sst>
 </file>
@@ -226,12 +246,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A584D702-F7C4-4DA2-BA32-09D8BB2C5F5D}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,59 +579,67 @@
     <col min="3" max="3" width="84.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>35</v>
@@ -619,133 +647,178 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2" t="s">
+      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2" t="s">
+      <c r="F9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A8:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Book shipment functionality half done
</commit_message>
<xml_diff>
--- a/Documentation/001-Requirement/API-List.xlsx
+++ b/Documentation/001-Requirement/API-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\001-Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD26C15-8E03-42B4-A051-BF27067CE5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C95E64-9E2B-495B-AE77-7FF064E41E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="11724" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Admin</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Create, Read, Update, Delete on Agent; 1 Stored Proc for Create and Update</t>
-  </si>
-  <si>
-    <t>Create, Read, Update, Delete on Customer; 1 Stored Proc for Create and Update</t>
   </si>
   <si>
     <t>Create, Read, Update, Delete on Employee; 1 Stored Proc for Create and Update; Create a sequence to generate employee_id of 6 digits</t>
@@ -179,6 +176,12 @@
   </si>
   <si>
     <t>shipment and shipment_tracker</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Customer; Upsert can be handled while booking shipment itself</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +645,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -657,7 +660,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -676,7 +679,9 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
@@ -736,7 +741,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
@@ -753,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
@@ -767,10 +772,10 @@
     <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>20</v>
@@ -784,10 +789,10 @@
     <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>20</v>
@@ -804,13 +809,13 @@
         <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>

</xml_diff>

<commit_message>
Implemented Receive and forward shipment API
</commit_message>
<xml_diff>
--- a/Documentation/001-Requirement/API-List.xlsx
+++ b/Documentation/001-Requirement/API-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\001-Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D61303-60F3-4383-8BC5-BF8C51263B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349252FD-14C2-4AC8-85E9-4B7AEF93AA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="11724" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Admin</t>
   </si>
@@ -274,9 +274,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,6 +285,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A584D702-F7C4-4DA2-BA32-09D8BB2C5F5D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +641,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -658,7 +658,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -673,7 +673,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -688,34 +688,34 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -729,119 +729,123 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Deliver shipment API implementation
</commit_message>
<xml_diff>
--- a/Documentation/001-Requirement/API-List.xlsx
+++ b/Documentation/001-Requirement/API-List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\001-Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349252FD-14C2-4AC8-85E9-4B7AEF93AA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4EB41C-9E59-4F1F-829C-2BAE7EF911EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Admin</t>
   </si>
@@ -157,34 +157,22 @@
     <t>Attempt Delivery</t>
   </si>
   <si>
-    <t>Update Delivery Status</t>
+    <t>At any point in time, customer should be able to track the full history of the shipment. This API would query shipment_tracker table and produce required output</t>
+  </si>
+  <si>
+    <t>shipment and shipment_tracker</t>
+  </si>
+  <si>
+    <t>Create, Read, Update, Delete on Customer; Upsert can be handled while booking shipment itself</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t xml:space="preserve">When a shipment is marked as RECEIVED_AT_DEST_BRANCH, an agent from the destination branch attempts the delivery and performs below task:
-1. Updates shipment table such that status = OUT_FOR_DELIVERY
-2. Insert a record into shipment_tracker; shipment_id, agent_id, creation_datetime,status=OUT_FOR_DELIVERY
+1. Updates shipment table such that status = OUT_FOR_DELIVERY or DELIVERED or UNDELIVERED
+2. Insert a record into shipment_tracker; shipment_id, agent_id, creation_datetime,status=OUT_FOR_DELIVERY or DELIVERED or UNDELIVERED
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When a shipment is marked as OUT_FOR_DELIVERY, the same agent from the destination branch updates the status of the delivery and performs below task:
-1. Updates shipment table such that status = DELIVERED or UNDELIVERED and adds status_remarks (optional)
-2. Insert a record into shipment_tracker; shipment_id, agent_id, creation_datetime,status=DELIVERED or UNDELIVERED
-</t>
-  </si>
-  <si>
-    <t>At any point in time, customer should be able to track the full history of the shipment. This API would query shipment_tracker table and produce required output</t>
-  </si>
-  <si>
-    <t>shipment and shipment_tracker</t>
-  </si>
-  <si>
-    <t>Create, Read, Update, Delete on Customer; Upsert can be handled while booking shipment itself</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -208,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,12 +212,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -280,10 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -603,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A584D702-F7C4-4DA2-BA32-09D8BB2C5F5D}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:G13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +619,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -658,7 +636,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -673,7 +651,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -688,12 +666,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -703,7 +681,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -713,7 +691,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>30</v>
@@ -729,7 +707,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -750,7 +728,7 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
@@ -769,7 +747,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
@@ -788,7 +766,7 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
@@ -807,64 +785,45 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A8:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Track shipment history API implemented
</commit_message>
<xml_diff>
--- a/Documentation/001-Requirement/API-List.xlsx
+++ b/Documentation/001-Requirement/API-List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\001-Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4EB41C-9E59-4F1F-829C-2BAE7EF911EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DB5F65-415B-4DC8-A0C6-9197936B15EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Admin</t>
   </si>
@@ -173,6 +173,10 @@
 1. Updates shipment table such that status = OUT_FOR_DELIVERY or DELIVERED or UNDELIVERED
 2. Insert a record into shipment_tracker; shipment_id, agent_id, creation_datetime,status=OUT_FOR_DELIVERY or DELIVERED or UNDELIVERED
 </t>
+  </si>
+  <si>
+    <t>SP Created; 
+Integration with Java code pending</t>
   </si>
 </sst>
 </file>
@@ -196,18 +200,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -260,12 +258,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A584D702-F7C4-4DA2-BA32-09D8BB2C5F5D}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,7 +591,7 @@
     <col min="3" max="3" width="84.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
     <col min="7" max="7" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -618,8 +616,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -630,13 +628,15 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -651,7 +651,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -666,34 +666,36 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -707,118 +709,120 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added Add Update Branch API which interacts with SP upsert_branch
</commit_message>
<xml_diff>
--- a/Documentation/001-Requirement/API-List.xlsx
+++ b/Documentation/001-Requirement/API-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\001-Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DB5F65-415B-4DC8-A0C6-9197936B15EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADF74E5-1A7E-42CE-82A6-59C46D9B5443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="11724" xr2:uid="{06D6A096-4748-4FD4-A1AA-E1DD8AC3B6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Admin</t>
   </si>
@@ -175,8 +175,12 @@
 </t>
   </si>
   <si>
-    <t>SP Created; 
-Integration with Java code pending</t>
+    <t>CU - Complete
+R - Pending</t>
+  </si>
+  <si>
+    <t>CU - SP Done; Calling Pending
+R - Pending</t>
   </si>
 </sst>
 </file>
@@ -258,12 +262,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,7 +586,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,8 +620,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -635,8 +639,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -645,13 +649,15 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -666,24 +672,24 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="9" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
@@ -709,120 +715,120 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>